<commit_message>
Updated output files to the August 2021 CRMMS ESP run
</commit_message>
<xml_diff>
--- a/Output Data/CrmmsToCrss_Annual.xlsx
+++ b/Output Data/CrmmsToCrss_Annual.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="798" uniqueCount="21">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>PowellOperation.Compact Point Volume</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
   <si>
     <t>SystemConditions.LBShortageTier</t>
@@ -827,7 +830,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -856,7 +859,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -874,10 +877,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -888,8 +891,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8353006.1438015867</v>
+      <c r="T2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -903,13 +906,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -918,19 +921,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>517992.49999999994</v>
       </c>
       <c r="I3">
-        <v>1019650.000000077</v>
+        <v>1032633.9999999242</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>286708.5</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -939,10 +942,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>969650.00000007695</v>
+        <v>982633.99999992421</v>
       </c>
       <c r="P3">
-        <v>505648.99999963935</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -954,7 +957,7 @@
         <v>2</v>
       </c>
       <c r="T3">
-        <v>7639775.9999999981</v>
+        <v>7635220.9999999981</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1028,7 +1031,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1057,7 +1060,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1075,10 +1078,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1089,8 +1092,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8373884.3098015878</v>
+      <c r="T2" s="69" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1104,13 +1107,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1119,19 +1122,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -1140,10 +1143,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1229,7 +1232,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1258,7 +1261,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1276,10 +1279,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1290,8 +1293,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8352616.3758015865</v>
+      <c r="T2" s="76" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1305,13 +1308,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1320,19 +1323,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -1341,22 +1344,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7150597.6699978551</v>
+        <v>7630597.6699999999</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1430,7 +1433,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1459,7 +1462,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1477,10 +1480,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1491,8 +1494,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8371082.8798015863</v>
+      <c r="T2" s="83" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1506,13 +1509,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1521,19 +1524,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1086212.5000007339</v>
+        <v>1159884.4000007345</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -1542,22 +1545,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1036212.5000007339</v>
+        <v>1109884.4000007345</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7136493.4259978561</v>
+        <v>7616493.425999999</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -1631,7 +1634,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1660,7 +1663,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1678,10 +1681,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1692,8 +1695,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8373055.0078015868</v>
+      <c r="T2" s="90" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1707,13 +1710,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1722,19 +1725,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -1743,10 +1746,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1832,7 +1835,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="98" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1861,7 +1864,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -1879,10 +1882,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1893,8 +1896,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8358449.8398015881</v>
+      <c r="T2" s="97" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1908,13 +1911,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1923,19 +1926,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -1944,10 +1947,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2033,7 +2036,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="105" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2062,7 +2065,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2080,10 +2083,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2094,8 +2097,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8382293.7618015874</v>
+      <c r="T2" s="104" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2109,13 +2112,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2124,19 +2127,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1304168.6999999066</v>
+        <v>1323395.3999999065</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -2145,22 +2148,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1254168.6999999066</v>
+        <v>1273395.3999999065</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8898225.943039922</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>9308044.1670399215</v>
+        <v>7889818.2239999976</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -2234,7 +2237,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="112" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2263,7 +2266,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2281,10 +2284,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2295,8 +2298,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8348966.5238015875</v>
+      <c r="T2" s="111" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2310,13 +2313,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2325,19 +2328,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -2346,10 +2349,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2435,7 +2438,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="119" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2464,7 +2467,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2482,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2496,8 +2499,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8345833.5898015862</v>
+      <c r="T2" s="118" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2511,13 +2514,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2526,19 +2529,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -2547,10 +2550,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2636,7 +2639,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2665,7 +2668,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2683,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2697,8 +2700,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8367655.9978015879</v>
+      <c r="T2" s="125" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2712,13 +2715,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2727,19 +2730,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -2748,10 +2751,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2837,7 +2840,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="133" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2866,7 +2869,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -2884,10 +2887,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2898,8 +2901,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8353658.3538015867</v>
+      <c r="T2" s="132" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2913,13 +2916,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2928,19 +2931,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -2949,10 +2952,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3038,7 +3041,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3067,7 +3070,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3085,10 +3088,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3099,8 +3102,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8359923.1438015876</v>
+      <c r="T2" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3114,13 +3117,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3129,19 +3132,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>517992.49999999994</v>
       </c>
       <c r="I3">
-        <v>1019650.000000077</v>
+        <v>1032633.9999999242</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>286708.5</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -3150,10 +3153,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>969650.00000007695</v>
+        <v>982633.99999992421</v>
       </c>
       <c r="P3">
-        <v>505648.99999963935</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3165,7 +3168,7 @@
         <v>2</v>
       </c>
       <c r="T3">
-        <v>7664230.9999999981</v>
+        <v>7692696.9999999972</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -3239,7 +3242,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="140" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3268,7 +3271,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3286,10 +3289,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3300,8 +3303,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8326850.4338015867</v>
+      <c r="T2" s="139" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3315,13 +3318,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3330,19 +3333,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -3351,10 +3354,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3440,7 +3443,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3469,7 +3472,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3487,10 +3490,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3501,8 +3504,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8326339.0238015866</v>
+      <c r="T2" s="146" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3516,13 +3519,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3531,19 +3534,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -3552,10 +3555,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3641,7 +3644,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="154" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3670,7 +3673,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3688,10 +3691,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3702,8 +3705,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8369143.6638015863</v>
+      <c r="T2" s="153" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3717,13 +3720,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3732,19 +3735,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1304168.6999999066</v>
+        <v>1323395.3999999065</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -3753,22 +3756,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1254168.6999999066</v>
+        <v>1273395.3999999065</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7140628.0299978545</v>
+        <v>7620628.0299999993</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -3842,7 +3845,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="161" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3871,7 +3874,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -3889,10 +3892,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3903,8 +3906,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8369540.2238015868</v>
+      <c r="T2" s="160" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3918,13 +3921,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3933,19 +3936,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -3954,10 +3957,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4043,7 +4046,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="168" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4072,7 +4075,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4090,10 +4093,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4104,8 +4107,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8332094.003801587</v>
+      <c r="T2" s="167" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4119,13 +4122,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4134,19 +4137,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -4155,22 +4158,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7108713.6499978546</v>
+        <v>7588713.6499999976</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -4244,7 +4247,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="175" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4273,7 +4276,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4291,10 +4294,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4305,8 +4308,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8355063.4338015877</v>
+      <c r="T2" s="174" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4320,13 +4323,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4335,19 +4338,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1304168.6999999066</v>
+        <v>1323395.3999999065</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -4356,10 +4359,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1254168.6999999066</v>
+        <v>1273395.3999999065</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4445,7 +4448,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="182" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4474,7 +4477,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4492,10 +4495,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4506,8 +4509,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8364742.0238015866</v>
+      <c r="T2" s="181" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4521,13 +4524,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4536,19 +4539,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -4557,22 +4560,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7104398.089997855</v>
+        <v>7584398.0899999989</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -4646,7 +4649,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="189" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4675,7 +4678,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4693,10 +4696,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4707,8 +4710,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8331859.8338015871</v>
+      <c r="T2" s="188" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4722,13 +4725,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4737,19 +4740,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1304168.6999999066</v>
+        <v>1323395.3999999065</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -4758,10 +4761,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1254168.6999999066</v>
+        <v>1273395.3999999065</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4847,7 +4850,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="196" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4876,7 +4879,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -4894,10 +4897,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4908,8 +4911,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8369657.8938015876</v>
+      <c r="T2" s="195" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4923,13 +4926,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4938,19 +4941,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -4959,10 +4962,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5048,7 +5051,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="203" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5077,7 +5080,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5095,10 +5098,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5109,8 +5112,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8404005.2238015868</v>
+      <c r="T2" s="202" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5124,13 +5127,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5139,19 +5142,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -5160,10 +5163,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5249,7 +5252,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5278,7 +5281,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5296,10 +5299,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5310,8 +5313,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8375472.1438015876</v>
+      <c r="T2" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5325,13 +5328,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>109360.60000000003</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5340,19 +5343,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>517992.49999999994</v>
       </c>
       <c r="I3">
-        <v>1019650.000000077</v>
+        <v>1032633.9999999242</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>286708.5</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -5361,10 +5364,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>969650.00000007695</v>
+        <v>982633.99999992421</v>
       </c>
       <c r="P3">
-        <v>505648.99999963935</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5450,7 +5453,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="210" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5479,7 +5482,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5497,10 +5500,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5511,8 +5514,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8353260.4038015865</v>
+      <c r="T2" s="209" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5526,13 +5529,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5541,19 +5544,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -5562,10 +5565,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5651,7 +5654,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="217" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5680,7 +5683,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5698,10 +5701,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5712,8 +5715,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8372247.6138015874</v>
+      <c r="T2" s="216" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5727,13 +5730,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5742,19 +5745,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -5763,22 +5766,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7524488.5246659201</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7684640.5946659194</v>
+        <v>7640152.0699999975</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -5852,7 +5855,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="224" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5881,7 +5884,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -5899,10 +5902,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5913,8 +5916,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8378639.4538015872</v>
+      <c r="T2" s="223" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5928,13 +5931,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5943,19 +5946,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -5964,22 +5967,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7183949.7199978568</v>
+        <v>7663949.7199999988</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -6053,7 +6056,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="231" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6082,7 +6085,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6100,10 +6103,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6114,8 +6117,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8365909.0838015862</v>
+      <c r="T2" s="230" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6129,13 +6132,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6144,19 +6147,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -6165,10 +6168,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6254,7 +6257,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="238" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6283,7 +6286,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6301,10 +6304,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6315,8 +6318,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8387384.6938015874</v>
+      <c r="T2" s="237" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6330,13 +6333,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6345,19 +6348,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -6366,10 +6369,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6455,7 +6458,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="245" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6484,7 +6487,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6502,10 +6505,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6516,8 +6519,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8325058.2438015873</v>
+      <c r="T2" s="244" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6531,13 +6534,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6546,19 +6549,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -6567,22 +6570,22 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>6999999.9999978552</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="S3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>7031744.7299978556</v>
+        <v>7511744.7299999986</v>
       </c>
       <c r="U3">
         <v>1</v>
@@ -6656,7 +6659,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="252" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6685,7 +6688,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6703,10 +6706,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6717,8 +6720,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8346963.2638015877</v>
+      <c r="T2" s="251" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6732,13 +6735,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6747,19 +6750,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -6768,10 +6771,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6857,7 +6860,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="259" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6886,7 +6889,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -6904,10 +6907,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6918,8 +6921,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8357801.8538015876</v>
+      <c r="T2" s="258" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6933,13 +6936,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6948,19 +6951,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>963433.00000000012</v>
+        <v>984796.00000000023</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -6969,10 +6972,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>913433.00000000012</v>
+        <v>934796.00000000012</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7058,7 +7061,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="266" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7087,7 +7090,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7105,10 +7108,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7119,8 +7122,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8365014.0738015873</v>
+      <c r="T2" s="265" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7134,13 +7137,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7149,19 +7152,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1086212.5000007339</v>
+        <v>1159884.4000007345</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -7170,10 +7173,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1036212.5000007339</v>
+        <v>1109884.4000007345</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7259,7 +7262,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7288,7 +7291,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7306,10 +7309,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7320,8 +7323,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8358287.5818015859</v>
+      <c r="T2" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7335,13 +7338,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7350,19 +7353,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -7371,10 +7374,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7460,7 +7463,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7489,7 +7492,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7507,10 +7510,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7521,8 +7524,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8373962.1638015872</v>
+      <c r="T2" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7536,13 +7539,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7551,19 +7554,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -7572,10 +7575,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7661,7 +7664,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7690,7 +7693,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7708,10 +7711,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7722,8 +7725,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8395964.3378015868</v>
+      <c r="T2" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7737,13 +7740,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7752,19 +7755,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -7773,10 +7776,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7862,7 +7865,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="49" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7891,7 +7894,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -7909,10 +7912,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7923,8 +7926,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8425252.6498015877</v>
+      <c r="T2" s="48" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7938,13 +7941,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7953,19 +7956,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -7974,10 +7977,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -8063,7 +8066,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -8092,7 +8095,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -8110,10 +8113,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -8124,8 +8127,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8338624.2358015878</v>
+      <c r="T2" s="55" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8139,13 +8142,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8154,19 +8157,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1439168.6999998132</v>
+        <v>1458395.3999998132</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -8175,10 +8178,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1389168.699999813</v>
+        <v>1408395.3999998132</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -8264,7 +8267,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -8293,7 +8296,7 @@
         <v>503067.5</v>
       </c>
       <c r="I2">
-        <v>1163433</v>
+        <v>1184796.0000000002</v>
       </c>
       <c r="J2">
         <v>273842</v>
@@ -8311,10 +8314,10 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>1113433</v>
+        <v>1134796</v>
       </c>
       <c r="P2">
-        <v>462348.99999981321</v>
+        <v>453348.99999981315</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -8325,8 +8328,8 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8329197.8998015868</v>
+      <c r="T2" s="62" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8340,13 +8343,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>59874.99999999853</v>
+        <v>54910.600000000013</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8355,19 +8358,19 @@
         <v>15999.999999999725</v>
       </c>
       <c r="H3">
-        <v>438184.00000000006</v>
+        <v>452248.39999999845</v>
       </c>
       <c r="I3">
-        <v>1063432.9999997991</v>
+        <v>1084795.9999997991</v>
       </c>
       <c r="J3">
-        <v>204742</v>
+        <v>213842</v>
       </c>
       <c r="K3">
         <v>17442</v>
       </c>
       <c r="L3">
-        <v>216000</v>
+        <v>220964.39999999845</v>
       </c>
       <c r="M3">
         <v>50000</v>
@@ -8376,10 +8379,10 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1013432.999999799</v>
+        <v>1034795.9999997991</v>
       </c>
       <c r="P3">
-        <v>482158.00000000029</v>
+        <v>487648.99999963929</v>
       </c>
       <c r="Q3">
         <v>0</v>

</xml_diff>